<commit_message>
Incorporating bat exogneous and endogenous taxa
</commit_message>
<xml_diff>
--- a/tabular/core/deltaretrovirus-reference-data.xlsx
+++ b/tabular/core/deltaretrovirus-reference-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/Retrovirus/Deltaretrovirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EC50E2-F353-6941-9F59-C12B9C229E39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586F5F0E-EB9D-EE4E-B8EF-E505C0449B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="920" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="41">
   <si>
     <t>Orthoretrovirinae</t>
   </si>
@@ -134,6 +134,21 @@
   </si>
   <si>
     <t>M10060</t>
+  </si>
+  <si>
+    <t>MT700539</t>
+  </si>
+  <si>
+    <t>EtDRV</t>
+  </si>
+  <si>
+    <t>Eptesicus fuscus deltaretrovirus</t>
+  </si>
+  <si>
+    <t>Eptesicus fuscus</t>
+  </si>
+  <si>
+    <t>Big brown bat</t>
   </si>
 </sst>
 </file>
@@ -1188,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I7" sqref="A1:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,6 +1394,35 @@
       </c>
       <c r="I6" s="4" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Misc updates. Added frameshifting features.
</commit_message>
<xml_diff>
--- a/tabular/core/deltaretrovirus-reference-data.xlsx
+++ b/tabular/core/deltaretrovirus-reference-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/Retrovirus/Deltaretrovirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AD3FB5-0FE5-3840-9A33-489E33206D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159A763D-C985-F440-852C-462AAF526F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="920" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="44">
   <si>
     <t>Orthoretrovirinae</t>
   </si>
@@ -151,7 +151,13 @@
     <t>Big brown bat</t>
   </si>
   <si>
-    <t>Cetartiodactyl</t>
+    <t>Chiroptera</t>
+  </si>
+  <si>
+    <t>Primates</t>
+  </si>
+  <si>
+    <t>Cetartiodactyla</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1215,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1274,7 +1280,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>20</v>
@@ -1303,7 +1309,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>19</v>
@@ -1332,7 +1338,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>19</v>
@@ -1361,7 +1367,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>19</v>
@@ -1389,8 +1395,8 @@
       <c r="F6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>26</v>
+      <c r="G6" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>19</v>
@@ -1419,7 +1425,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Updated feature locations (frameshifting features)
</commit_message>
<xml_diff>
--- a/tabular/core/deltaretrovirus-reference-data.xlsx
+++ b/tabular/core/deltaretrovirus-reference-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/Retrovirus/Deltaretrovirus-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159A763D-C985-F440-852C-462AAF526F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46943FF-9B1D-7A4C-899B-A8FDA74D59F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3200" yWindow="920" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>